<commit_message>
updated bbox for axis and california removed excess axis images
</commit_message>
<xml_diff>
--- a/multi_stage_ocr/results/handwritten_results/cmparison.xlsx
+++ b/multi_stage_ocr/results/handwritten_results/cmparison.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Kare4U\ocr\multi_stage_ocr\results\handwritten_results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C716E652-5346-4F7B-9706-741879856D32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{3F9D812F-93CF-4FFD-83A0-DDF49424C2FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720"/>
   </bookViews>
@@ -133,9 +133,6 @@
     <t xml:space="preserve"> Marit April The</t>
   </si>
   <si>
-    <t xml:space="preserve"> SUNIL</t>
-  </si>
-  <si>
     <t>137a.png</t>
   </si>
   <si>
@@ -752,6 +749,9 @@
   </si>
   <si>
     <t xml:space="preserve"> Premaid Reagan.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -1636,7 +1636,7 @@
   <dimension ref="A1:G61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1785,27 +1785,27 @@
         <v>36</v>
       </c>
       <c r="G6" t="s">
-        <v>37</v>
+        <v>243</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" t="s">
         <v>38</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="D7" t="s">
         <v>40</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>41</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>42</v>
-      </c>
-      <c r="F7" t="s">
-        <v>43</v>
       </c>
       <c r="G7" t="s">
         <v>13</v>
@@ -1813,68 +1813,68 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B8" t="s">
         <v>44</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D8" t="s">
         <v>45</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
+        <v>44</v>
+      </c>
+      <c r="F8" t="s">
         <v>46</v>
       </c>
-      <c r="E8" t="s">
-        <v>45</v>
-      </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>47</v>
-      </c>
-      <c r="G8" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B9" t="s">
         <v>49</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="D9" t="s">
         <v>51</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="F9" t="s">
         <v>53</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>54</v>
-      </c>
-      <c r="G9" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="B10" t="s">
         <v>56</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="D10" t="s">
         <v>58</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="F10" t="s">
         <v>60</v>
-      </c>
-      <c r="F10" t="s">
-        <v>61</v>
       </c>
       <c r="G10" t="s">
         <v>13</v>
@@ -1882,45 +1882,45 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B11" t="s">
         <v>62</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="D11" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E11" t="s">
         <v>64</v>
       </c>
-      <c r="D11" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>65</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
         <v>66</v>
-      </c>
-      <c r="G11" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="B12" t="s">
         <v>68</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="D12" t="s">
         <v>70</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>71</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
         <v>72</v>
-      </c>
-      <c r="F12" t="s">
-        <v>73</v>
       </c>
       <c r="G12" t="s">
         <v>13</v>
@@ -1928,22 +1928,22 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="B13" t="s">
         <v>74</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>75</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>76</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>77</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
         <v>78</v>
-      </c>
-      <c r="F13" t="s">
-        <v>79</v>
       </c>
       <c r="G13" t="s">
         <v>13</v>
@@ -1951,22 +1951,22 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="B14" t="s">
         <v>80</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="D14" t="s">
         <v>82</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>83</v>
       </c>
-      <c r="E14" t="s">
+      <c r="F14" t="s">
         <v>84</v>
-      </c>
-      <c r="F14" t="s">
-        <v>85</v>
       </c>
       <c r="G14" t="s">
         <v>13</v>
@@ -1974,22 +1974,22 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="B15" t="s">
         <v>86</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="D15" t="s">
         <v>88</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="E15" s="5" t="s">
+      <c r="F15" t="s">
         <v>90</v>
-      </c>
-      <c r="F15" t="s">
-        <v>91</v>
       </c>
       <c r="G15" t="s">
         <v>13</v>
@@ -1997,22 +1997,22 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="B16" t="s">
         <v>92</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
         <v>93</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="E16" t="s">
+        <v>93</v>
+      </c>
+      <c r="F16" t="s">
         <v>95</v>
-      </c>
-      <c r="E16" t="s">
-        <v>94</v>
-      </c>
-      <c r="F16" t="s">
-        <v>96</v>
       </c>
       <c r="G16" t="s">
         <v>13</v>
@@ -2020,22 +2020,22 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="B17" t="s">
         <v>97</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="D17" t="s">
         <v>99</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E17" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="F17" t="s">
         <v>100</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="F17" t="s">
-        <v>101</v>
       </c>
       <c r="G17" t="s">
         <v>13</v>
@@ -2043,68 +2043,68 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="B18" t="s">
         <v>102</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="D18" t="s">
         <v>104</v>
       </c>
-      <c r="D18" t="s">
+      <c r="E18" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="F18" t="s">
         <v>105</v>
       </c>
-      <c r="E18" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="F18" t="s">
+      <c r="G18" t="s">
         <v>106</v>
-      </c>
-      <c r="G18" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="B19" t="s">
         <v>108</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="C19" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="D19" s="1" t="s">
+      <c r="E19" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="F19" t="s">
         <v>110</v>
       </c>
-      <c r="E19" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="F19" t="s">
+      <c r="G19" t="s">
         <v>111</v>
-      </c>
-      <c r="G19" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="B20" t="s">
         <v>113</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="C20" s="5" t="s">
+      <c r="D20" t="s">
         <v>115</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
         <v>116</v>
       </c>
-      <c r="E20" t="s">
+      <c r="F20" t="s">
         <v>117</v>
-      </c>
-      <c r="F20" t="s">
-        <v>118</v>
       </c>
       <c r="G20" t="s">
         <v>13</v>
@@ -2112,22 +2112,22 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="B21" t="s">
         <v>119</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C21" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="D21" t="s">
         <v>121</v>
       </c>
-      <c r="D21" t="s">
+      <c r="E21" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="F21" t="s">
         <v>122</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="F21" t="s">
-        <v>123</v>
       </c>
       <c r="G21" t="s">
         <v>13</v>
@@ -2135,22 +2135,22 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="B22" t="s">
         <v>124</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C22" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D22" t="s">
         <v>125</v>
       </c>
-      <c r="C22" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="D22" t="s">
+      <c r="E22" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="F22" t="s">
         <v>126</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="F22" t="s">
-        <v>127</v>
       </c>
       <c r="G22" t="s">
         <v>13</v>
@@ -2158,114 +2158,114 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="B23" t="s">
         <v>128</v>
       </c>
-      <c r="B23" t="s">
+      <c r="C23" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="D23" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="D23" s="1" t="s">
+      <c r="E23" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="F23" t="s">
         <v>131</v>
       </c>
-      <c r="E23" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="F23" t="s">
+      <c r="G23" t="s">
         <v>132</v>
-      </c>
-      <c r="G23" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="B24" t="s">
         <v>134</v>
       </c>
-      <c r="B24" t="s">
+      <c r="C24" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="D24" t="s">
         <v>135</v>
       </c>
-      <c r="C24" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="D24" t="s">
+      <c r="E24" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="F24" t="s">
         <v>136</v>
       </c>
-      <c r="E24" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="F24" t="s">
+      <c r="G24" t="s">
         <v>137</v>
-      </c>
-      <c r="G24" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="B25" t="s">
         <v>139</v>
       </c>
-      <c r="B25" t="s">
+      <c r="C25" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="D25" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="C25" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="D25" s="1" t="s">
+      <c r="E25" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="F25" t="s">
         <v>141</v>
       </c>
-      <c r="E25" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="F25" t="s">
+      <c r="G25" t="s">
         <v>142</v>
-      </c>
-      <c r="G25" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="B26" t="s">
         <v>144</v>
       </c>
-      <c r="B26" t="s">
+      <c r="C26" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="D26" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="D26" s="1" t="s">
+      <c r="E26" t="s">
         <v>147</v>
       </c>
-      <c r="E26" t="s">
+      <c r="F26" t="s">
         <v>148</v>
       </c>
-      <c r="F26" t="s">
+      <c r="G26" t="s">
         <v>149</v>
-      </c>
-      <c r="G26" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="B27" t="s">
         <v>151</v>
       </c>
-      <c r="B27" t="s">
+      <c r="C27" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="D27" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="C27" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="D27" s="1" t="s">
+      <c r="E27" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="E27" s="1" t="s">
+      <c r="F27" t="s">
         <v>154</v>
-      </c>
-      <c r="F27" t="s">
-        <v>155</v>
       </c>
       <c r="G27" t="s">
         <v>13</v>
@@ -2273,366 +2273,366 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="B28" t="s">
         <v>160</v>
       </c>
-      <c r="B28" t="s">
-        <v>161</v>
-      </c>
       <c r="C28" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E28" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="B29" t="s">
         <v>162</v>
       </c>
-      <c r="B29" t="s">
-        <v>163</v>
-      </c>
       <c r="C29" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E29" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="B30" t="s">
         <v>164</v>
       </c>
-      <c r="B30" t="s">
-        <v>165</v>
-      </c>
       <c r="C30" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D30" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E30" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="B31" t="s">
         <v>166</v>
       </c>
-      <c r="B31" t="s">
-        <v>167</v>
-      </c>
       <c r="C31" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D31" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E31" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="B32" t="s">
         <v>168</v>
       </c>
-      <c r="B32" t="s">
-        <v>169</v>
-      </c>
       <c r="C32" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D32" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E32" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="B33" t="s">
         <v>170</v>
       </c>
-      <c r="B33" t="s">
-        <v>171</v>
-      </c>
       <c r="C33" s="5" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D33" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E33" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="B34" t="s">
         <v>172</v>
       </c>
-      <c r="B34" t="s">
-        <v>173</v>
-      </c>
       <c r="C34" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="B35" t="s">
         <v>174</v>
       </c>
-      <c r="B35" t="s">
-        <v>175</v>
-      </c>
       <c r="C35" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D35" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E35" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B36" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D36" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E36" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="B37" t="s">
         <v>177</v>
       </c>
-      <c r="B37" t="s">
-        <v>178</v>
-      </c>
       <c r="C37" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="B38" t="s">
         <v>179</v>
       </c>
-      <c r="B38" t="s">
-        <v>180</v>
-      </c>
       <c r="C38" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D38" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E38" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
+        <v>180</v>
+      </c>
+      <c r="B39" t="s">
         <v>181</v>
       </c>
-      <c r="B39" t="s">
-        <v>182</v>
-      </c>
       <c r="C39" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="B40" t="s">
         <v>183</v>
       </c>
-      <c r="B40" t="s">
-        <v>184</v>
-      </c>
       <c r="C40" s="5" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D40" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E40" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
+        <v>184</v>
+      </c>
+      <c r="B41" t="s">
         <v>185</v>
       </c>
-      <c r="B41" t="s">
-        <v>186</v>
-      </c>
       <c r="C41" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E41" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="6" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B42" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="6" t="s">
+        <v>225</v>
+      </c>
+      <c r="B43" t="s">
         <v>226</v>
       </c>
-      <c r="B43" t="s">
-        <v>227</v>
-      </c>
       <c r="C43" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D43" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E43" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="6" t="s">
+        <v>227</v>
+      </c>
+      <c r="B44" t="s">
         <v>228</v>
       </c>
-      <c r="B44" t="s">
-        <v>229</v>
-      </c>
       <c r="C44" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="6" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B45" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D45" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="B46" t="s">
         <v>231</v>
       </c>
-      <c r="B46" t="s">
-        <v>232</v>
-      </c>
       <c r="C46" s="5" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D46" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="6" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B47" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D47" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E47" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="58" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D58" s="5"/>
       <c r="E58" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="59" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D59" s="1"/>
       <c r="E59" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="60" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D60" s="2"/>
       <c r="E60" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="61" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D61" s="4"/>
       <c r="E61" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
   </sheetData>

</xml_diff>